<commit_message>
Updated sample trading application
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t>CCY1</t>
   </si>
@@ -215,16 +215,20 @@
   </si>
   <si>
     <t>Model.BaseAmount</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +275,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +319,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
       </patternFill>
     </fill>
   </fills>
@@ -322,10 +351,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -374,9 +404,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -385,10 +412,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="40" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -397,16 +420,27 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFAED9C3"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFAED9C3"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFFFF"/>
     </mruColors>
@@ -420,6 +454,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,7 +477,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="ExcelMvc.ManualDeal"/>
+        <xdr:cNvPr id="6" name="ExcelMvc.Command.ManualDeal"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -515,19 +553,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:colOff>1114425</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="ExcelMvc.AutoDeal"/>
+        <xdr:cNvPr id="9" name="ExcelMvc.Command.AutoDeal"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2847975" y="400048"/>
-          <a:ext cx="1019175" cy="533402"/>
+          <a:ext cx="1057275" cy="533402"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -562,7 +600,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -613,7 +651,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="ExcelMvc.AutoRate"/>
+        <xdr:cNvPr id="4" name="ExcelMvc.Command.AutoRate"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -654,7 +692,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
@@ -733,7 +771,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="ExcelMvc.Reset"/>
+        <xdr:cNvPr id="7" name="ExcelMvc.Command.Reset"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -795,6 +833,89 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="absolute">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>57150</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>38100</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>85725</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>266700</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="ExcelMvc.Command.InsideMode" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FF9900" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="52"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="7F7F7F"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Inside Trading</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -1084,12 +1205,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,15 +1242,19 @@
       <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-    </row>
-    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="21"/>
+      <c r="C3" s="22"/>
+      <c r="E3" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
@@ -1142,7 +1267,7 @@
       <c r="D8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="26">
         <f>SUM(E10:E100)</f>
         <v>0</v>
       </c>
@@ -1151,13 +1276,13 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="15" t="s">
@@ -1166,7 +1291,7 @@
       <c r="E9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="15" t="s">
@@ -1177,737 +1302,737 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="G10" s="20" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="G10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <v>0.92</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <v>0.92</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="G11" s="20" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="G11" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="20">
         <v>102.4</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <v>102.4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="G12" s="20" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="G12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <v>1.68</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <v>1.68</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="G13" s="20" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="G13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="20">
         <v>1.37</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <v>1.37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="G14" s="20" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="G14" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="20">
         <v>6.24</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="20">
         <v>6.24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="G15" s="20" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="G15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="20">
         <v>7.75</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <v>7.75</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
+      <c r="A52" s="25"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
+      <c r="A55" s="25"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="25"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
+      <c r="A56" s="25"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="25"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="A57" s="25"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
+      <c r="A59" s="25"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
+      <c r="A60" s="25"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
+      <c r="A61" s="25"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
+      <c r="A62" s="25"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
+      <c r="D62" s="25"/>
+      <c r="E62" s="25"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
+      <c r="D63" s="25"/>
+      <c r="E63" s="25"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="20"/>
+      <c r="A64" s="25"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
+      <c r="D64" s="25"/>
+      <c r="E64" s="25"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
+      <c r="A66" s="25"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
+      <c r="A67" s="25"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
+      <c r="A68" s="25"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="25"/>
+      <c r="E68" s="25"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
+      <c r="A69" s="25"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="25"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
+      <c r="A70" s="25"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="25"/>
+      <c r="E70" s="25"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
+      <c r="A71" s="25"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
+      <c r="A72" s="25"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
+      <c r="A73" s="25"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="25"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
+      <c r="A74" s="25"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
+      <c r="A75" s="25"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="25"/>
+      <c r="E75" s="25"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
+      <c r="A76" s="25"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
+      <c r="A77" s="25"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
+      <c r="A78" s="25"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="25"/>
+      <c r="E78" s="25"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
+      <c r="A79" s="25"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
+      <c r="A80" s="25"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
+      <c r="A81" s="25"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="25"/>
+      <c r="E81" s="25"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="25"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="25"/>
+      <c r="E82" s="25"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
+      <c r="A83" s="25"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="25"/>
+      <c r="E83" s="25"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
+      <c r="A84" s="25"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="25"/>
+      <c r="E84" s="25"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
+      <c r="A85" s="25"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="25"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
-      <c r="E86" s="20"/>
+      <c r="A86" s="25"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="20"/>
+      <c r="A87" s="25"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="20"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="20"/>
+      <c r="A88" s="25"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="20"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="20"/>
+      <c r="A89" s="25"/>
+      <c r="B89" s="25"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="25"/>
+      <c r="E89" s="25"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="20"/>
-      <c r="D90" s="20"/>
-      <c r="E90" s="20"/>
+      <c r="A90" s="25"/>
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="25"/>
+      <c r="E90" s="25"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="20"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
+      <c r="A91" s="25"/>
+      <c r="B91" s="25"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="25"/>
+      <c r="E91" s="25"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
+      <c r="A92" s="25"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="25"/>
+      <c r="E92" s="25"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="20"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
+      <c r="A93" s="25"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="20"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
+      <c r="A94" s="25"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="25"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="20"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
+      <c r="A95" s="25"/>
+      <c r="B95" s="25"/>
+      <c r="C95" s="25"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="25"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="20"/>
-      <c r="D96" s="20"/>
-      <c r="E96" s="20"/>
+      <c r="A96" s="25"/>
+      <c r="B96" s="25"/>
+      <c r="C96" s="25"/>
+      <c r="D96" s="25"/>
+      <c r="E96" s="25"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
+      <c r="A97" s="25"/>
+      <c r="B97" s="25"/>
+      <c r="C97" s="25"/>
+      <c r="D97" s="25"/>
+      <c r="E97" s="25"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="20"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="20"/>
+      <c r="A98" s="25"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="25"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="20"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="20"/>
+      <c r="A99" s="25"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="25"/>
+      <c r="D99" s="25"/>
+      <c r="E99" s="25"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="20"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
-      <c r="E100" s="20"/>
+      <c r="A100" s="25"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="25"/>
+      <c r="D100" s="25"/>
+      <c r="E100" s="25"/>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" s="13">
@@ -1915,9 +2040,39 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="ExcelMvc.Command.InsideMode">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor>
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>38100</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>5</xdr:col>
+                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>266700</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Completed Sample Trading application. Needs Context switch for the message window
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="-45" windowWidth="20565" windowHeight="9270"/>
+    <workbookView xWindow="630" yWindow="-45" windowWidth="20565" windowHeight="9270" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Trading" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="59">
   <si>
     <t>CCY1</t>
   </si>
@@ -164,24 +164,6 @@
   </si>
   <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t>AUD/USD</t>
-  </si>
-  <si>
-    <t>USD/JPY</t>
-  </si>
-  <si>
-    <t>GBP/USD</t>
-  </si>
-  <si>
-    <t>EUR/USD</t>
-  </si>
-  <si>
-    <t>USD/CNY</t>
-  </si>
-  <si>
-    <t>USD/HKD</t>
   </si>
   <si>
     <t>Deal Form</t>
@@ -427,9 +409,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -475,7 +455,7 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>127125</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="ExcelMvc.Command.ManualDeal"/>
         <xdr:cNvSpPr/>
@@ -557,7 +537,7 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="9" name="ExcelMvc.Command.AutoDeal"/>
         <xdr:cNvSpPr/>
@@ -649,7 +629,7 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171452</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="ExcelMvc.Command.AutoRate"/>
         <xdr:cNvSpPr/>
@@ -769,7 +749,7 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>127125</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp macro="ExcelMvcRunCommandAction" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="ExcelMvc.Command.Reset"/>
         <xdr:cNvSpPr/>
@@ -1208,9 +1188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1207,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1243,9 +1223,11 @@
         <v>5</v>
       </c>
       <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
+      <c r="C3" s="22">
+        <v>0</v>
+      </c>
       <c r="E3" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1253,7 +1235,9 @@
         <v>6</v>
       </c>
       <c r="B4" s="21"/>
-      <c r="C4" s="22"/>
+      <c r="C4" s="22">
+        <v>0</v>
+      </c>
       <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1262,7 +1246,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>4</v>
@@ -1307,15 +1291,9 @@
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
-      <c r="G10" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="20">
-        <v>0.92</v>
-      </c>
-      <c r="I10" s="20">
-        <v>0.92</v>
-      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
@@ -1323,15 +1301,9 @@
       <c r="C11" s="24"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
-      <c r="G11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="20">
-        <v>102.4</v>
-      </c>
-      <c r="I11" s="20">
-        <v>102.4</v>
-      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
@@ -1339,15 +1311,9 @@
       <c r="C12" s="24"/>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
-      <c r="G12" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="20">
-        <v>1.68</v>
-      </c>
-      <c r="I12" s="20">
-        <v>1.68</v>
-      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
@@ -1355,15 +1321,9 @@
       <c r="C13" s="24"/>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
-      <c r="G13" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="20">
-        <v>1.37</v>
-      </c>
-      <c r="I13" s="20">
-        <v>1.37</v>
-      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
@@ -1371,15 +1331,9 @@
       <c r="C14" s="24"/>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
-      <c r="G14" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="20">
-        <v>6.24</v>
-      </c>
-      <c r="I14" s="20">
-        <v>6.24</v>
-      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
@@ -1387,15 +1341,9 @@
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
-      <c r="G15" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="H15" s="20">
-        <v>7.75</v>
-      </c>
-      <c r="I15" s="20">
-        <v>7.75</v>
-      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
@@ -2051,7 +1999,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1026" r:id="rId4" name="ExcelMvc.Command.InsideMode">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" macro="ExcelMvcRunCommandAction">
                 <anchor>
                   <from>
                     <xdr:col>4</xdr:col>
@@ -2073,6 +2021,24 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$F$4:$F$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$F$4:$F$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2321,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2590,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2633,7 +2599,7 @@
         <v>[SpotTrading.xlsx]Trading!$A$10</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>27</v>
@@ -2642,7 +2608,10 @@
         <v>36</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="str">
+        <f ca="1">CELL("address", Trading!A100)</f>
+        <v>[SpotTrading.xlsx]Trading!$A$100</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="str">
@@ -2650,7 +2619,7 @@
         <v>[SpotTrading.xlsx]Trading!$B$10</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>27</v>
@@ -2659,7 +2628,10 @@
         <v>36</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="str">
+        <f ca="1">CELL("address", Trading!B100)</f>
+        <v>[SpotTrading.xlsx]Trading!$B$100</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="str">
@@ -2667,7 +2639,7 @@
         <v>[SpotTrading.xlsx]Trading!$C$10</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>27</v>
@@ -2676,7 +2648,10 @@
         <v>36</v>
       </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="str">
+        <f ca="1">CELL("address", Trading!C100)</f>
+        <v>[SpotTrading.xlsx]Trading!$C$100</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="str">
@@ -2684,7 +2659,7 @@
         <v>[SpotTrading.xlsx]Trading!$D$10</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>27</v>
@@ -2693,7 +2668,10 @@
         <v>36</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="str">
+        <f ca="1">CELL("address", Trading!D100)</f>
+        <v>[SpotTrading.xlsx]Trading!$D$100</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="str">
@@ -2701,7 +2679,7 @@
         <v>[SpotTrading.xlsx]Trading!$E$10</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>27</v>
@@ -2710,7 +2688,10 @@
         <v>36</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="str">
+        <f ca="1">CELL("address", Trading!E100)</f>
+        <v>[SpotTrading.xlsx]Trading!$E$100</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2756,7 +2737,7 @@
         <v>[SpotTrading.xlsx]Trading!$B$3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>33</v>
@@ -2776,7 +2757,7 @@
         <v>[SpotTrading.xlsx]Trading!$C$3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>33</v>
@@ -2793,7 +2774,7 @@
         <v>[SpotTrading.xlsx]Trading!$B$4</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>33</v>
@@ -2813,7 +2794,7 @@
         <v>[SpotTrading.xlsx]Trading!$C$4</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Updated Sample Trading Applications. Needs to investigate RaiseChanged on table row. Extremely slow.
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="-45" windowWidth="20565" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="630" yWindow="-45" windowWidth="20565" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Trading" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00;0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -405,11 +406,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -1186,11 +1187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I400"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1252,7 @@
       <c r="D8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="24">
         <f>SUM(E10:E100)</f>
         <v>0</v>
       </c>
@@ -1286,709 +1287,2803 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
       <c r="G10" s="19"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="G12" s="19"/>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
       <c r="I17" s="20"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
       <c r="I19" s="20"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
       <c r="G20" s="19"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
       <c r="G21" s="19"/>
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
       <c r="G22" s="19"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
       <c r="G23" s="19"/>
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
       <c r="G24" s="19"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
       <c r="G25" s="19"/>
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="G26" s="19"/>
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
       <c r="I27" s="20"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
       <c r="I28" s="20"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="26"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="26"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="25"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
+      <c r="A61" s="26"/>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="25"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="26"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="25"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="25"/>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="25"/>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="26"/>
+      <c r="D66" s="26"/>
+      <c r="E66" s="26"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="25"/>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="26"/>
+      <c r="D67" s="26"/>
+      <c r="E67" s="26"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="25"/>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
+      <c r="A69" s="26"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="25"/>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="25"/>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="26"/>
+      <c r="E71" s="26"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="25"/>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="26"/>
+      <c r="D72" s="26"/>
+      <c r="E72" s="26"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="25"/>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="26"/>
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="25"/>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="26"/>
+      <c r="D74" s="26"/>
+      <c r="E74" s="26"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="25"/>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="25"/>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="26"/>
+      <c r="D76" s="26"/>
+      <c r="E76" s="26"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="25"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
+      <c r="A77" s="26"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="26"/>
+      <c r="D77" s="26"/>
+      <c r="E77" s="26"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="25"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
+      <c r="A78" s="26"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
+      <c r="D78" s="26"/>
+      <c r="E78" s="26"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
+      <c r="A79" s="26"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
+      <c r="D79" s="26"/>
+      <c r="E79" s="26"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
+      <c r="A80" s="26"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
+      <c r="D80" s="26"/>
+      <c r="E80" s="26"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="25"/>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
+      <c r="D81" s="26"/>
+      <c r="E81" s="26"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="25"/>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="26"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="25"/>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
+      <c r="A83" s="26"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="D83" s="26"/>
+      <c r="E83" s="26"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="25"/>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="25"/>
-      <c r="B85" s="25"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="25"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="25"/>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
+      <c r="A88" s="26"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="25"/>
-      <c r="B89" s="25"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
+      <c r="A89" s="26"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
+      <c r="D89" s="26"/>
+      <c r="E89" s="26"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="25"/>
-      <c r="B90" s="25"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
+      <c r="A90" s="26"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
+      <c r="D90" s="26"/>
+      <c r="E90" s="26"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="25"/>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
+      <c r="D91" s="26"/>
+      <c r="E91" s="26"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="25"/>
-      <c r="B92" s="25"/>
-      <c r="C92" s="25"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
+      <c r="A92" s="26"/>
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
+      <c r="D92" s="26"/>
+      <c r="E92" s="26"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="25"/>
-      <c r="B93" s="25"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
+      <c r="A93" s="26"/>
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
+      <c r="D93" s="26"/>
+      <c r="E93" s="26"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="25"/>
-      <c r="B94" s="25"/>
-      <c r="C94" s="25"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="25"/>
-      <c r="B95" s="25"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
+      <c r="A95" s="26"/>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
+      <c r="D95" s="26"/>
+      <c r="E95" s="26"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="25"/>
-      <c r="B96" s="25"/>
-      <c r="C96" s="25"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="26"/>
+      <c r="C96" s="26"/>
+      <c r="D96" s="26"/>
+      <c r="E96" s="26"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="25"/>
-      <c r="B97" s="25"/>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
+      <c r="A97" s="26"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
+      <c r="D97" s="26"/>
+      <c r="E97" s="26"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="25"/>
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
+      <c r="A98" s="26"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="26"/>
+      <c r="D98" s="26"/>
+      <c r="E98" s="26"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="25"/>
-      <c r="B99" s="25"/>
-      <c r="C99" s="25"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
+      <c r="A99" s="26"/>
+      <c r="B99" s="26"/>
+      <c r="C99" s="26"/>
+      <c r="D99" s="26"/>
+      <c r="E99" s="26"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="25"/>
-      <c r="B100" s="25"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-    </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="13">
-        <v>333</v>
-      </c>
+      <c r="A100" s="26"/>
+      <c r="B100" s="26"/>
+      <c r="C100" s="26"/>
+      <c r="D100" s="26"/>
+      <c r="E100" s="26"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="26"/>
+      <c r="B101" s="26"/>
+      <c r="C101" s="26"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="26"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="26"/>
+      <c r="B102" s="26"/>
+      <c r="C102" s="26"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="26"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="26"/>
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="26"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="26"/>
+      <c r="B104" s="26"/>
+      <c r="C104" s="26"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="26"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="26"/>
+      <c r="B105" s="26"/>
+      <c r="C105" s="26"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="26"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="26"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="26"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="26"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="26"/>
+      <c r="B107" s="26"/>
+      <c r="C107" s="26"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="26"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="26"/>
+      <c r="B108" s="26"/>
+      <c r="C108" s="26"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="26"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="26"/>
+      <c r="B109" s="26"/>
+      <c r="C109" s="26"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="26"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="26"/>
+      <c r="B110" s="26"/>
+      <c r="C110" s="26"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="26"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="26"/>
+      <c r="B111" s="26"/>
+      <c r="C111" s="26"/>
+      <c r="D111" s="26"/>
+      <c r="E111" s="26"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="26"/>
+      <c r="B112" s="26"/>
+      <c r="C112" s="26"/>
+      <c r="D112" s="26"/>
+      <c r="E112" s="26"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="26"/>
+      <c r="B113" s="26"/>
+      <c r="C113" s="26"/>
+      <c r="D113" s="26"/>
+      <c r="E113" s="26"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="26"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="26"/>
+      <c r="D114" s="26"/>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="26"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="26"/>
+      <c r="D115" s="26"/>
+      <c r="E115" s="26"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="26"/>
+      <c r="B116" s="26"/>
+      <c r="C116" s="26"/>
+      <c r="D116" s="26"/>
+      <c r="E116" s="26"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="26"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="26"/>
+      <c r="E117" s="26"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="26"/>
+      <c r="B118" s="26"/>
+      <c r="C118" s="26"/>
+      <c r="D118" s="26"/>
+      <c r="E118" s="26"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="26"/>
+      <c r="B119" s="26"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="26"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="26"/>
+      <c r="B120" s="26"/>
+      <c r="C120" s="26"/>
+      <c r="D120" s="26"/>
+      <c r="E120" s="26"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="26"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="26"/>
+      <c r="D121" s="26"/>
+      <c r="E121" s="26"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="26"/>
+      <c r="B122" s="26"/>
+      <c r="C122" s="26"/>
+      <c r="D122" s="26"/>
+      <c r="E122" s="26"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="26"/>
+      <c r="B123" s="26"/>
+      <c r="C123" s="26"/>
+      <c r="D123" s="26"/>
+      <c r="E123" s="26"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="26"/>
+      <c r="B124" s="26"/>
+      <c r="C124" s="26"/>
+      <c r="D124" s="26"/>
+      <c r="E124" s="26"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="26"/>
+      <c r="B125" s="26"/>
+      <c r="C125" s="26"/>
+      <c r="D125" s="26"/>
+      <c r="E125" s="26"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="26"/>
+      <c r="B126" s="26"/>
+      <c r="C126" s="26"/>
+      <c r="D126" s="26"/>
+      <c r="E126" s="26"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="26"/>
+      <c r="B127" s="26"/>
+      <c r="C127" s="26"/>
+      <c r="D127" s="26"/>
+      <c r="E127" s="26"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="26"/>
+      <c r="B128" s="26"/>
+      <c r="C128" s="26"/>
+      <c r="D128" s="26"/>
+      <c r="E128" s="26"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="26"/>
+      <c r="B129" s="26"/>
+      <c r="C129" s="26"/>
+      <c r="D129" s="26"/>
+      <c r="E129" s="26"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="26"/>
+      <c r="B130" s="26"/>
+      <c r="C130" s="26"/>
+      <c r="D130" s="26"/>
+      <c r="E130" s="26"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="26"/>
+      <c r="B131" s="26"/>
+      <c r="C131" s="26"/>
+      <c r="D131" s="26"/>
+      <c r="E131" s="26"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="26"/>
+      <c r="B132" s="26"/>
+      <c r="C132" s="26"/>
+      <c r="D132" s="26"/>
+      <c r="E132" s="26"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="26"/>
+      <c r="B133" s="26"/>
+      <c r="C133" s="26"/>
+      <c r="D133" s="26"/>
+      <c r="E133" s="26"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="26"/>
+      <c r="B134" s="26"/>
+      <c r="C134" s="26"/>
+      <c r="D134" s="26"/>
+      <c r="E134" s="26"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="26"/>
+      <c r="B135" s="26"/>
+      <c r="C135" s="26"/>
+      <c r="D135" s="26"/>
+      <c r="E135" s="26"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="26"/>
+      <c r="B136" s="26"/>
+      <c r="C136" s="26"/>
+      <c r="D136" s="26"/>
+      <c r="E136" s="26"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="26"/>
+      <c r="B137" s="26"/>
+      <c r="C137" s="26"/>
+      <c r="D137" s="26"/>
+      <c r="E137" s="26"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="26"/>
+      <c r="B138" s="26"/>
+      <c r="C138" s="26"/>
+      <c r="D138" s="26"/>
+      <c r="E138" s="26"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="26"/>
+      <c r="B139" s="26"/>
+      <c r="C139" s="26"/>
+      <c r="D139" s="26"/>
+      <c r="E139" s="26"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="26"/>
+      <c r="B140" s="26"/>
+      <c r="C140" s="26"/>
+      <c r="D140" s="26"/>
+      <c r="E140" s="26"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="26"/>
+      <c r="B141" s="26"/>
+      <c r="C141" s="26"/>
+      <c r="D141" s="26"/>
+      <c r="E141" s="26"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="26"/>
+      <c r="B142" s="26"/>
+      <c r="C142" s="26"/>
+      <c r="D142" s="26"/>
+      <c r="E142" s="26"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="26"/>
+      <c r="B143" s="26"/>
+      <c r="C143" s="26"/>
+      <c r="D143" s="26"/>
+      <c r="E143" s="26"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="26"/>
+      <c r="B144" s="26"/>
+      <c r="C144" s="26"/>
+      <c r="D144" s="26"/>
+      <c r="E144" s="26"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="26"/>
+      <c r="B145" s="26"/>
+      <c r="C145" s="26"/>
+      <c r="D145" s="26"/>
+      <c r="E145" s="26"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="26"/>
+      <c r="B146" s="26"/>
+      <c r="C146" s="26"/>
+      <c r="D146" s="26"/>
+      <c r="E146" s="26"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="26"/>
+      <c r="B147" s="26"/>
+      <c r="C147" s="26"/>
+      <c r="D147" s="26"/>
+      <c r="E147" s="26"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="26"/>
+      <c r="B148" s="26"/>
+      <c r="C148" s="26"/>
+      <c r="D148" s="26"/>
+      <c r="E148" s="26"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="26"/>
+      <c r="B149" s="26"/>
+      <c r="C149" s="26"/>
+      <c r="D149" s="26"/>
+      <c r="E149" s="26"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="26"/>
+      <c r="B150" s="26"/>
+      <c r="C150" s="26"/>
+      <c r="D150" s="26"/>
+      <c r="E150" s="26"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="26"/>
+      <c r="B151" s="26"/>
+      <c r="C151" s="26"/>
+      <c r="D151" s="26"/>
+      <c r="E151" s="26"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="26"/>
+      <c r="B152" s="26"/>
+      <c r="C152" s="26"/>
+      <c r="D152" s="26"/>
+      <c r="E152" s="26"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="26"/>
+      <c r="B153" s="26"/>
+      <c r="C153" s="26"/>
+      <c r="D153" s="26"/>
+      <c r="E153" s="26"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="26"/>
+      <c r="B154" s="26"/>
+      <c r="C154" s="26"/>
+      <c r="D154" s="26"/>
+      <c r="E154" s="26"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="26"/>
+      <c r="B155" s="26"/>
+      <c r="C155" s="26"/>
+      <c r="D155" s="26"/>
+      <c r="E155" s="26"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="26"/>
+      <c r="B156" s="26"/>
+      <c r="C156" s="26"/>
+      <c r="D156" s="26"/>
+      <c r="E156" s="26"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="26"/>
+      <c r="B157" s="26"/>
+      <c r="C157" s="26"/>
+      <c r="D157" s="26"/>
+      <c r="E157" s="26"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="26"/>
+      <c r="B158" s="26"/>
+      <c r="C158" s="26"/>
+      <c r="D158" s="26"/>
+      <c r="E158" s="26"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="26"/>
+      <c r="B159" s="26"/>
+      <c r="C159" s="26"/>
+      <c r="D159" s="26"/>
+      <c r="E159" s="26"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="26"/>
+      <c r="B160" s="26"/>
+      <c r="C160" s="26"/>
+      <c r="D160" s="26"/>
+      <c r="E160" s="26"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="26"/>
+      <c r="B161" s="26"/>
+      <c r="C161" s="26"/>
+      <c r="D161" s="26"/>
+      <c r="E161" s="26"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="26"/>
+      <c r="B162" s="26"/>
+      <c r="C162" s="26"/>
+      <c r="D162" s="26"/>
+      <c r="E162" s="26"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="26"/>
+      <c r="B163" s="26"/>
+      <c r="C163" s="26"/>
+      <c r="D163" s="26"/>
+      <c r="E163" s="26"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="26"/>
+      <c r="B164" s="26"/>
+      <c r="C164" s="26"/>
+      <c r="D164" s="26"/>
+      <c r="E164" s="26"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="26"/>
+      <c r="B165" s="26"/>
+      <c r="C165" s="26"/>
+      <c r="D165" s="26"/>
+      <c r="E165" s="26"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="26"/>
+      <c r="B166" s="26"/>
+      <c r="C166" s="26"/>
+      <c r="D166" s="26"/>
+      <c r="E166" s="26"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="26"/>
+      <c r="B167" s="26"/>
+      <c r="C167" s="26"/>
+      <c r="D167" s="26"/>
+      <c r="E167" s="26"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="26"/>
+      <c r="B168" s="26"/>
+      <c r="C168" s="26"/>
+      <c r="D168" s="26"/>
+      <c r="E168" s="26"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="26"/>
+      <c r="B169" s="26"/>
+      <c r="C169" s="26"/>
+      <c r="D169" s="26"/>
+      <c r="E169" s="26"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="26"/>
+      <c r="B170" s="26"/>
+      <c r="C170" s="26"/>
+      <c r="D170" s="26"/>
+      <c r="E170" s="26"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="26"/>
+      <c r="B171" s="26"/>
+      <c r="C171" s="26"/>
+      <c r="D171" s="26"/>
+      <c r="E171" s="26"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="26"/>
+      <c r="B172" s="26"/>
+      <c r="C172" s="26"/>
+      <c r="D172" s="26"/>
+      <c r="E172" s="26"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="26"/>
+      <c r="B173" s="26"/>
+      <c r="C173" s="26"/>
+      <c r="D173" s="26"/>
+      <c r="E173" s="26"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="26"/>
+      <c r="B174" s="26"/>
+      <c r="C174" s="26"/>
+      <c r="D174" s="26"/>
+      <c r="E174" s="26"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="26"/>
+      <c r="B175" s="26"/>
+      <c r="C175" s="26"/>
+      <c r="D175" s="26"/>
+      <c r="E175" s="26"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="26"/>
+      <c r="B176" s="26"/>
+      <c r="C176" s="26"/>
+      <c r="D176" s="26"/>
+      <c r="E176" s="26"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="26"/>
+      <c r="B177" s="26"/>
+      <c r="C177" s="26"/>
+      <c r="D177" s="26"/>
+      <c r="E177" s="26"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="26"/>
+      <c r="B178" s="26"/>
+      <c r="C178" s="26"/>
+      <c r="D178" s="26"/>
+      <c r="E178" s="26"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="26"/>
+      <c r="B179" s="26"/>
+      <c r="C179" s="26"/>
+      <c r="D179" s="26"/>
+      <c r="E179" s="26"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="26"/>
+      <c r="B180" s="26"/>
+      <c r="C180" s="26"/>
+      <c r="D180" s="26"/>
+      <c r="E180" s="26"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="26"/>
+      <c r="B181" s="26"/>
+      <c r="C181" s="26"/>
+      <c r="D181" s="26"/>
+      <c r="E181" s="26"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="26"/>
+      <c r="B182" s="26"/>
+      <c r="C182" s="26"/>
+      <c r="D182" s="26"/>
+      <c r="E182" s="26"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="26"/>
+      <c r="B183" s="26"/>
+      <c r="C183" s="26"/>
+      <c r="D183" s="26"/>
+      <c r="E183" s="26"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="26"/>
+      <c r="B184" s="26"/>
+      <c r="C184" s="26"/>
+      <c r="D184" s="26"/>
+      <c r="E184" s="26"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="26"/>
+      <c r="B185" s="26"/>
+      <c r="C185" s="26"/>
+      <c r="D185" s="26"/>
+      <c r="E185" s="26"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="26"/>
+      <c r="B186" s="26"/>
+      <c r="C186" s="26"/>
+      <c r="D186" s="26"/>
+      <c r="E186" s="26"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="26"/>
+      <c r="B187" s="26"/>
+      <c r="C187" s="26"/>
+      <c r="D187" s="26"/>
+      <c r="E187" s="26"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="26"/>
+      <c r="B188" s="26"/>
+      <c r="C188" s="26"/>
+      <c r="D188" s="26"/>
+      <c r="E188" s="26"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="26"/>
+      <c r="B189" s="26"/>
+      <c r="C189" s="26"/>
+      <c r="D189" s="26"/>
+      <c r="E189" s="26"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="26"/>
+      <c r="B190" s="26"/>
+      <c r="C190" s="26"/>
+      <c r="D190" s="26"/>
+      <c r="E190" s="26"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="26"/>
+      <c r="B191" s="26"/>
+      <c r="C191" s="26"/>
+      <c r="D191" s="26"/>
+      <c r="E191" s="26"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="26"/>
+      <c r="B192" s="26"/>
+      <c r="C192" s="26"/>
+      <c r="D192" s="26"/>
+      <c r="E192" s="26"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="26"/>
+      <c r="B193" s="26"/>
+      <c r="C193" s="26"/>
+      <c r="D193" s="26"/>
+      <c r="E193" s="26"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="26"/>
+      <c r="B194" s="26"/>
+      <c r="C194" s="26"/>
+      <c r="D194" s="26"/>
+      <c r="E194" s="26"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="26"/>
+      <c r="B195" s="26"/>
+      <c r="C195" s="26"/>
+      <c r="D195" s="26"/>
+      <c r="E195" s="26"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="26"/>
+      <c r="B196" s="26"/>
+      <c r="C196" s="26"/>
+      <c r="D196" s="26"/>
+      <c r="E196" s="26"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="26"/>
+      <c r="B197" s="26"/>
+      <c r="C197" s="26"/>
+      <c r="D197" s="26"/>
+      <c r="E197" s="26"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="26"/>
+      <c r="B198" s="26"/>
+      <c r="C198" s="26"/>
+      <c r="D198" s="26"/>
+      <c r="E198" s="26"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="26"/>
+      <c r="B199" s="26"/>
+      <c r="C199" s="26"/>
+      <c r="D199" s="26"/>
+      <c r="E199" s="26"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="26"/>
+      <c r="B200" s="26"/>
+      <c r="C200" s="26"/>
+      <c r="D200" s="26"/>
+      <c r="E200" s="26"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="26"/>
+      <c r="B201" s="26"/>
+      <c r="C201" s="26"/>
+      <c r="D201" s="26"/>
+      <c r="E201" s="26"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="26"/>
+      <c r="B202" s="26"/>
+      <c r="C202" s="26"/>
+      <c r="D202" s="26"/>
+      <c r="E202" s="26"/>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="26"/>
+      <c r="B203" s="26"/>
+      <c r="C203" s="26"/>
+      <c r="D203" s="26"/>
+      <c r="E203" s="26"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="26"/>
+      <c r="B204" s="26"/>
+      <c r="C204" s="26"/>
+      <c r="D204" s="26"/>
+      <c r="E204" s="26"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="26"/>
+      <c r="B205" s="26"/>
+      <c r="C205" s="26"/>
+      <c r="D205" s="26"/>
+      <c r="E205" s="26"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="26"/>
+      <c r="B206" s="26"/>
+      <c r="C206" s="26"/>
+      <c r="D206" s="26"/>
+      <c r="E206" s="26"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="26"/>
+      <c r="B207" s="26"/>
+      <c r="C207" s="26"/>
+      <c r="D207" s="26"/>
+      <c r="E207" s="26"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="26"/>
+      <c r="B208" s="26"/>
+      <c r="C208" s="26"/>
+      <c r="D208" s="26"/>
+      <c r="E208" s="26"/>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="26"/>
+      <c r="B209" s="26"/>
+      <c r="C209" s="26"/>
+      <c r="D209" s="26"/>
+      <c r="E209" s="26"/>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="26"/>
+      <c r="B210" s="26"/>
+      <c r="C210" s="26"/>
+      <c r="D210" s="26"/>
+      <c r="E210" s="26"/>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="26"/>
+      <c r="B211" s="26"/>
+      <c r="C211" s="26"/>
+      <c r="D211" s="26"/>
+      <c r="E211" s="26"/>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="26"/>
+      <c r="B212" s="26"/>
+      <c r="C212" s="26"/>
+      <c r="D212" s="26"/>
+      <c r="E212" s="26"/>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="26"/>
+      <c r="B213" s="26"/>
+      <c r="C213" s="26"/>
+      <c r="D213" s="26"/>
+      <c r="E213" s="26"/>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="26"/>
+      <c r="B214" s="26"/>
+      <c r="C214" s="26"/>
+      <c r="D214" s="26"/>
+      <c r="E214" s="26"/>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="26"/>
+      <c r="B215" s="26"/>
+      <c r="C215" s="26"/>
+      <c r="D215" s="26"/>
+      <c r="E215" s="26"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="26"/>
+      <c r="B216" s="26"/>
+      <c r="C216" s="26"/>
+      <c r="D216" s="26"/>
+      <c r="E216" s="26"/>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="26"/>
+      <c r="B217" s="26"/>
+      <c r="C217" s="26"/>
+      <c r="D217" s="26"/>
+      <c r="E217" s="26"/>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="26"/>
+      <c r="B218" s="26"/>
+      <c r="C218" s="26"/>
+      <c r="D218" s="26"/>
+      <c r="E218" s="26"/>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="26"/>
+      <c r="B219" s="26"/>
+      <c r="C219" s="26"/>
+      <c r="D219" s="26"/>
+      <c r="E219" s="26"/>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="26"/>
+      <c r="B220" s="26"/>
+      <c r="C220" s="26"/>
+      <c r="D220" s="26"/>
+      <c r="E220" s="26"/>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="26"/>
+      <c r="B221" s="26"/>
+      <c r="C221" s="26"/>
+      <c r="D221" s="26"/>
+      <c r="E221" s="26"/>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="26"/>
+      <c r="B222" s="26"/>
+      <c r="C222" s="26"/>
+      <c r="D222" s="26"/>
+      <c r="E222" s="26"/>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="26"/>
+      <c r="B223" s="26"/>
+      <c r="C223" s="26"/>
+      <c r="D223" s="26"/>
+      <c r="E223" s="26"/>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="26"/>
+      <c r="B224" s="26"/>
+      <c r="C224" s="26"/>
+      <c r="D224" s="26"/>
+      <c r="E224" s="26"/>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="26"/>
+      <c r="B225" s="26"/>
+      <c r="C225" s="26"/>
+      <c r="D225" s="26"/>
+      <c r="E225" s="26"/>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="26"/>
+      <c r="B226" s="26"/>
+      <c r="C226" s="26"/>
+      <c r="D226" s="26"/>
+      <c r="E226" s="26"/>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="26"/>
+      <c r="B227" s="26"/>
+      <c r="C227" s="26"/>
+      <c r="D227" s="26"/>
+      <c r="E227" s="26"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="26"/>
+      <c r="B228" s="26"/>
+      <c r="C228" s="26"/>
+      <c r="D228" s="26"/>
+      <c r="E228" s="26"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="26"/>
+      <c r="B229" s="26"/>
+      <c r="C229" s="26"/>
+      <c r="D229" s="26"/>
+      <c r="E229" s="26"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="26"/>
+      <c r="B230" s="26"/>
+      <c r="C230" s="26"/>
+      <c r="D230" s="26"/>
+      <c r="E230" s="26"/>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="26"/>
+      <c r="B231" s="26"/>
+      <c r="C231" s="26"/>
+      <c r="D231" s="26"/>
+      <c r="E231" s="26"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="26"/>
+      <c r="B232" s="26"/>
+      <c r="C232" s="26"/>
+      <c r="D232" s="26"/>
+      <c r="E232" s="26"/>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="26"/>
+      <c r="B233" s="26"/>
+      <c r="C233" s="26"/>
+      <c r="D233" s="26"/>
+      <c r="E233" s="26"/>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="26"/>
+      <c r="B234" s="26"/>
+      <c r="C234" s="26"/>
+      <c r="D234" s="26"/>
+      <c r="E234" s="26"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="26"/>
+      <c r="B235" s="26"/>
+      <c r="C235" s="26"/>
+      <c r="D235" s="26"/>
+      <c r="E235" s="26"/>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="26"/>
+      <c r="B236" s="26"/>
+      <c r="C236" s="26"/>
+      <c r="D236" s="26"/>
+      <c r="E236" s="26"/>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="26"/>
+      <c r="B237" s="26"/>
+      <c r="C237" s="26"/>
+      <c r="D237" s="26"/>
+      <c r="E237" s="26"/>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="26"/>
+      <c r="B238" s="26"/>
+      <c r="C238" s="26"/>
+      <c r="D238" s="26"/>
+      <c r="E238" s="26"/>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="26"/>
+      <c r="B239" s="26"/>
+      <c r="C239" s="26"/>
+      <c r="D239" s="26"/>
+      <c r="E239" s="26"/>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="26"/>
+      <c r="B240" s="26"/>
+      <c r="C240" s="26"/>
+      <c r="D240" s="26"/>
+      <c r="E240" s="26"/>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="26"/>
+      <c r="B241" s="26"/>
+      <c r="C241" s="26"/>
+      <c r="D241" s="26"/>
+      <c r="E241" s="26"/>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="26"/>
+      <c r="B242" s="26"/>
+      <c r="C242" s="26"/>
+      <c r="D242" s="26"/>
+      <c r="E242" s="26"/>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="26"/>
+      <c r="B243" s="26"/>
+      <c r="C243" s="26"/>
+      <c r="D243" s="26"/>
+      <c r="E243" s="26"/>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="26"/>
+      <c r="B244" s="26"/>
+      <c r="C244" s="26"/>
+      <c r="D244" s="26"/>
+      <c r="E244" s="26"/>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="26"/>
+      <c r="B245" s="26"/>
+      <c r="C245" s="26"/>
+      <c r="D245" s="26"/>
+      <c r="E245" s="26"/>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="26"/>
+      <c r="B246" s="26"/>
+      <c r="C246" s="26"/>
+      <c r="D246" s="26"/>
+      <c r="E246" s="26"/>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="26"/>
+      <c r="B247" s="26"/>
+      <c r="C247" s="26"/>
+      <c r="D247" s="26"/>
+      <c r="E247" s="26"/>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="26"/>
+      <c r="B248" s="26"/>
+      <c r="C248" s="26"/>
+      <c r="D248" s="26"/>
+      <c r="E248" s="26"/>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="26"/>
+      <c r="B249" s="26"/>
+      <c r="C249" s="26"/>
+      <c r="D249" s="26"/>
+      <c r="E249" s="26"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="26"/>
+      <c r="B250" s="26"/>
+      <c r="C250" s="26"/>
+      <c r="D250" s="26"/>
+      <c r="E250" s="26"/>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="26"/>
+      <c r="B251" s="26"/>
+      <c r="C251" s="26"/>
+      <c r="D251" s="26"/>
+      <c r="E251" s="26"/>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="26"/>
+      <c r="B252" s="26"/>
+      <c r="C252" s="26"/>
+      <c r="D252" s="26"/>
+      <c r="E252" s="26"/>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="26"/>
+      <c r="B253" s="26"/>
+      <c r="C253" s="26"/>
+      <c r="D253" s="26"/>
+      <c r="E253" s="26"/>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="26"/>
+      <c r="B254" s="26"/>
+      <c r="C254" s="26"/>
+      <c r="D254" s="26"/>
+      <c r="E254" s="26"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="26"/>
+      <c r="B255" s="26"/>
+      <c r="C255" s="26"/>
+      <c r="D255" s="26"/>
+      <c r="E255" s="26"/>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="26"/>
+      <c r="B256" s="26"/>
+      <c r="C256" s="26"/>
+      <c r="D256" s="26"/>
+      <c r="E256" s="26"/>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="26"/>
+      <c r="B257" s="26"/>
+      <c r="C257" s="26"/>
+      <c r="D257" s="26"/>
+      <c r="E257" s="26"/>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="26"/>
+      <c r="B258" s="26"/>
+      <c r="C258" s="26"/>
+      <c r="D258" s="26"/>
+      <c r="E258" s="26"/>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A259" s="26"/>
+      <c r="B259" s="26"/>
+      <c r="C259" s="26"/>
+      <c r="D259" s="26"/>
+      <c r="E259" s="26"/>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A260" s="26"/>
+      <c r="B260" s="26"/>
+      <c r="C260" s="26"/>
+      <c r="D260" s="26"/>
+      <c r="E260" s="26"/>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A261" s="26"/>
+      <c r="B261" s="26"/>
+      <c r="C261" s="26"/>
+      <c r="D261" s="26"/>
+      <c r="E261" s="26"/>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A262" s="26"/>
+      <c r="B262" s="26"/>
+      <c r="C262" s="26"/>
+      <c r="D262" s="26"/>
+      <c r="E262" s="26"/>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A263" s="26"/>
+      <c r="B263" s="26"/>
+      <c r="C263" s="26"/>
+      <c r="D263" s="26"/>
+      <c r="E263" s="26"/>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A264" s="26"/>
+      <c r="B264" s="26"/>
+      <c r="C264" s="26"/>
+      <c r="D264" s="26"/>
+      <c r="E264" s="26"/>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A265" s="26"/>
+      <c r="B265" s="26"/>
+      <c r="C265" s="26"/>
+      <c r="D265" s="26"/>
+      <c r="E265" s="26"/>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A266" s="26"/>
+      <c r="B266" s="26"/>
+      <c r="C266" s="26"/>
+      <c r="D266" s="26"/>
+      <c r="E266" s="26"/>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A267" s="26"/>
+      <c r="B267" s="26"/>
+      <c r="C267" s="26"/>
+      <c r="D267" s="26"/>
+      <c r="E267" s="26"/>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A268" s="26"/>
+      <c r="B268" s="26"/>
+      <c r="C268" s="26"/>
+      <c r="D268" s="26"/>
+      <c r="E268" s="26"/>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A269" s="26"/>
+      <c r="B269" s="26"/>
+      <c r="C269" s="26"/>
+      <c r="D269" s="26"/>
+      <c r="E269" s="26"/>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A270" s="26"/>
+      <c r="B270" s="26"/>
+      <c r="C270" s="26"/>
+      <c r="D270" s="26"/>
+      <c r="E270" s="26"/>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A271" s="26"/>
+      <c r="B271" s="26"/>
+      <c r="C271" s="26"/>
+      <c r="D271" s="26"/>
+      <c r="E271" s="26"/>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A272" s="26"/>
+      <c r="B272" s="26"/>
+      <c r="C272" s="26"/>
+      <c r="D272" s="26"/>
+      <c r="E272" s="26"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="26"/>
+      <c r="B273" s="26"/>
+      <c r="C273" s="26"/>
+      <c r="D273" s="26"/>
+      <c r="E273" s="26"/>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A274" s="26"/>
+      <c r="B274" s="26"/>
+      <c r="C274" s="26"/>
+      <c r="D274" s="26"/>
+      <c r="E274" s="26"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A275" s="26"/>
+      <c r="B275" s="26"/>
+      <c r="C275" s="26"/>
+      <c r="D275" s="26"/>
+      <c r="E275" s="26"/>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A276" s="26"/>
+      <c r="B276" s="26"/>
+      <c r="C276" s="26"/>
+      <c r="D276" s="26"/>
+      <c r="E276" s="26"/>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A277" s="26"/>
+      <c r="B277" s="26"/>
+      <c r="C277" s="26"/>
+      <c r="D277" s="26"/>
+      <c r="E277" s="26"/>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A278" s="26"/>
+      <c r="B278" s="26"/>
+      <c r="C278" s="26"/>
+      <c r="D278" s="26"/>
+      <c r="E278" s="26"/>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A279" s="26"/>
+      <c r="B279" s="26"/>
+      <c r="C279" s="26"/>
+      <c r="D279" s="26"/>
+      <c r="E279" s="26"/>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A280" s="26"/>
+      <c r="B280" s="26"/>
+      <c r="C280" s="26"/>
+      <c r="D280" s="26"/>
+      <c r="E280" s="26"/>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A281" s="26"/>
+      <c r="B281" s="26"/>
+      <c r="C281" s="26"/>
+      <c r="D281" s="26"/>
+      <c r="E281" s="26"/>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A282" s="26"/>
+      <c r="B282" s="26"/>
+      <c r="C282" s="26"/>
+      <c r="D282" s="26"/>
+      <c r="E282" s="26"/>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A283" s="26"/>
+      <c r="B283" s="26"/>
+      <c r="C283" s="26"/>
+      <c r="D283" s="26"/>
+      <c r="E283" s="26"/>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A284" s="26"/>
+      <c r="B284" s="26"/>
+      <c r="C284" s="26"/>
+      <c r="D284" s="26"/>
+      <c r="E284" s="26"/>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A285" s="26"/>
+      <c r="B285" s="26"/>
+      <c r="C285" s="26"/>
+      <c r="D285" s="26"/>
+      <c r="E285" s="26"/>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A286" s="26"/>
+      <c r="B286" s="26"/>
+      <c r="C286" s="26"/>
+      <c r="D286" s="26"/>
+      <c r="E286" s="26"/>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A287" s="26"/>
+      <c r="B287" s="26"/>
+      <c r="C287" s="26"/>
+      <c r="D287" s="26"/>
+      <c r="E287" s="26"/>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A288" s="26"/>
+      <c r="B288" s="26"/>
+      <c r="C288" s="26"/>
+      <c r="D288" s="26"/>
+      <c r="E288" s="26"/>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A289" s="26"/>
+      <c r="B289" s="26"/>
+      <c r="C289" s="26"/>
+      <c r="D289" s="26"/>
+      <c r="E289" s="26"/>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A290" s="26"/>
+      <c r="B290" s="26"/>
+      <c r="C290" s="26"/>
+      <c r="D290" s="26"/>
+      <c r="E290" s="26"/>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A291" s="26"/>
+      <c r="B291" s="26"/>
+      <c r="C291" s="26"/>
+      <c r="D291" s="26"/>
+      <c r="E291" s="26"/>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A292" s="26"/>
+      <c r="B292" s="26"/>
+      <c r="C292" s="26"/>
+      <c r="D292" s="26"/>
+      <c r="E292" s="26"/>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A293" s="26"/>
+      <c r="B293" s="26"/>
+      <c r="C293" s="26"/>
+      <c r="D293" s="26"/>
+      <c r="E293" s="26"/>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A294" s="26"/>
+      <c r="B294" s="26"/>
+      <c r="C294" s="26"/>
+      <c r="D294" s="26"/>
+      <c r="E294" s="26"/>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A295" s="26"/>
+      <c r="B295" s="26"/>
+      <c r="C295" s="26"/>
+      <c r="D295" s="26"/>
+      <c r="E295" s="26"/>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A296" s="26"/>
+      <c r="B296" s="26"/>
+      <c r="C296" s="26"/>
+      <c r="D296" s="26"/>
+      <c r="E296" s="26"/>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A297" s="26"/>
+      <c r="B297" s="26"/>
+      <c r="C297" s="26"/>
+      <c r="D297" s="26"/>
+      <c r="E297" s="26"/>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A298" s="26"/>
+      <c r="B298" s="26"/>
+      <c r="C298" s="26"/>
+      <c r="D298" s="26"/>
+      <c r="E298" s="26"/>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A299" s="26"/>
+      <c r="B299" s="26"/>
+      <c r="C299" s="26"/>
+      <c r="D299" s="26"/>
+      <c r="E299" s="26"/>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A300" s="26"/>
+      <c r="B300" s="26"/>
+      <c r="C300" s="26"/>
+      <c r="D300" s="26"/>
+      <c r="E300" s="26"/>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A301" s="26"/>
+      <c r="B301" s="26"/>
+      <c r="C301" s="26"/>
+      <c r="D301" s="26"/>
+      <c r="E301" s="26"/>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A302" s="26"/>
+      <c r="B302" s="26"/>
+      <c r="C302" s="26"/>
+      <c r="D302" s="26"/>
+      <c r="E302" s="26"/>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A303" s="26"/>
+      <c r="B303" s="26"/>
+      <c r="C303" s="26"/>
+      <c r="D303" s="26"/>
+      <c r="E303" s="26"/>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A304" s="26"/>
+      <c r="B304" s="26"/>
+      <c r="C304" s="26"/>
+      <c r="D304" s="26"/>
+      <c r="E304" s="26"/>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A305" s="26"/>
+      <c r="B305" s="26"/>
+      <c r="C305" s="26"/>
+      <c r="D305" s="26"/>
+      <c r="E305" s="26"/>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A306" s="26"/>
+      <c r="B306" s="26"/>
+      <c r="C306" s="26"/>
+      <c r="D306" s="26"/>
+      <c r="E306" s="26"/>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A307" s="26"/>
+      <c r="B307" s="26"/>
+      <c r="C307" s="26"/>
+      <c r="D307" s="26"/>
+      <c r="E307" s="26"/>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A308" s="26"/>
+      <c r="B308" s="26"/>
+      <c r="C308" s="26"/>
+      <c r="D308" s="26"/>
+      <c r="E308" s="26"/>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A309" s="26"/>
+      <c r="B309" s="26"/>
+      <c r="C309" s="26"/>
+      <c r="D309" s="26"/>
+      <c r="E309" s="26"/>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A310" s="26"/>
+      <c r="B310" s="26"/>
+      <c r="C310" s="26"/>
+      <c r="D310" s="26"/>
+      <c r="E310" s="26"/>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A311" s="26"/>
+      <c r="B311" s="26"/>
+      <c r="C311" s="26"/>
+      <c r="D311" s="26"/>
+      <c r="E311" s="26"/>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A312" s="26"/>
+      <c r="B312" s="26"/>
+      <c r="C312" s="26"/>
+      <c r="D312" s="26"/>
+      <c r="E312" s="26"/>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A313" s="26"/>
+      <c r="B313" s="26"/>
+      <c r="C313" s="26"/>
+      <c r="D313" s="26"/>
+      <c r="E313" s="26"/>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A314" s="26"/>
+      <c r="B314" s="26"/>
+      <c r="C314" s="26"/>
+      <c r="D314" s="26"/>
+      <c r="E314" s="26"/>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A315" s="26"/>
+      <c r="B315" s="26"/>
+      <c r="C315" s="26"/>
+      <c r="D315" s="26"/>
+      <c r="E315" s="26"/>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A316" s="26"/>
+      <c r="B316" s="26"/>
+      <c r="C316" s="26"/>
+      <c r="D316" s="26"/>
+      <c r="E316" s="26"/>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A317" s="26"/>
+      <c r="B317" s="26"/>
+      <c r="C317" s="26"/>
+      <c r="D317" s="26"/>
+      <c r="E317" s="26"/>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A318" s="26"/>
+      <c r="B318" s="26"/>
+      <c r="C318" s="26"/>
+      <c r="D318" s="26"/>
+      <c r="E318" s="26"/>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A319" s="26"/>
+      <c r="B319" s="26"/>
+      <c r="C319" s="26"/>
+      <c r="D319" s="26"/>
+      <c r="E319" s="26"/>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A320" s="26"/>
+      <c r="B320" s="26"/>
+      <c r="C320" s="26"/>
+      <c r="D320" s="26"/>
+      <c r="E320" s="26"/>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A321" s="26"/>
+      <c r="B321" s="26"/>
+      <c r="C321" s="26"/>
+      <c r="D321" s="26"/>
+      <c r="E321" s="26"/>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A322" s="26"/>
+      <c r="B322" s="26"/>
+      <c r="C322" s="26"/>
+      <c r="D322" s="26"/>
+      <c r="E322" s="26"/>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A323" s="26"/>
+      <c r="B323" s="26"/>
+      <c r="C323" s="26"/>
+      <c r="D323" s="26"/>
+      <c r="E323" s="26"/>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A324" s="26"/>
+      <c r="B324" s="26"/>
+      <c r="C324" s="26"/>
+      <c r="D324" s="26"/>
+      <c r="E324" s="26"/>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A325" s="26"/>
+      <c r="B325" s="26"/>
+      <c r="C325" s="26"/>
+      <c r="D325" s="26"/>
+      <c r="E325" s="26"/>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A326" s="26"/>
+      <c r="B326" s="26"/>
+      <c r="C326" s="26"/>
+      <c r="D326" s="26"/>
+      <c r="E326" s="26"/>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A327" s="26"/>
+      <c r="B327" s="26"/>
+      <c r="C327" s="26"/>
+      <c r="D327" s="26"/>
+      <c r="E327" s="26"/>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A328" s="26"/>
+      <c r="B328" s="26"/>
+      <c r="C328" s="26"/>
+      <c r="D328" s="26"/>
+      <c r="E328" s="26"/>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A329" s="26"/>
+      <c r="B329" s="26"/>
+      <c r="C329" s="26"/>
+      <c r="D329" s="26"/>
+      <c r="E329" s="26"/>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A330" s="26"/>
+      <c r="B330" s="26"/>
+      <c r="C330" s="26"/>
+      <c r="D330" s="26"/>
+      <c r="E330" s="26"/>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A331" s="26"/>
+      <c r="B331" s="26"/>
+      <c r="C331" s="26"/>
+      <c r="D331" s="26"/>
+      <c r="E331" s="26"/>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A332" s="26"/>
+      <c r="B332" s="26"/>
+      <c r="C332" s="26"/>
+      <c r="D332" s="26"/>
+      <c r="E332" s="26"/>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A333" s="26"/>
+      <c r="B333" s="26"/>
+      <c r="C333" s="26"/>
+      <c r="D333" s="26"/>
+      <c r="E333" s="26"/>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A334" s="26"/>
+      <c r="B334" s="26"/>
+      <c r="C334" s="26"/>
+      <c r="D334" s="26"/>
+      <c r="E334" s="26"/>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A335" s="26"/>
+      <c r="B335" s="26"/>
+      <c r="C335" s="26"/>
+      <c r="D335" s="26"/>
+      <c r="E335" s="26"/>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A336" s="26"/>
+      <c r="B336" s="26"/>
+      <c r="C336" s="26"/>
+      <c r="D336" s="26"/>
+      <c r="E336" s="26"/>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A337" s="26"/>
+      <c r="B337" s="26"/>
+      <c r="C337" s="26"/>
+      <c r="D337" s="26"/>
+      <c r="E337" s="26"/>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A338" s="26"/>
+      <c r="B338" s="26"/>
+      <c r="C338" s="26"/>
+      <c r="D338" s="26"/>
+      <c r="E338" s="26"/>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A339" s="26"/>
+      <c r="B339" s="26"/>
+      <c r="C339" s="26"/>
+      <c r="D339" s="26"/>
+      <c r="E339" s="26"/>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A340" s="26"/>
+      <c r="B340" s="26"/>
+      <c r="C340" s="26"/>
+      <c r="D340" s="26"/>
+      <c r="E340" s="26"/>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A341" s="26"/>
+      <c r="B341" s="26"/>
+      <c r="C341" s="26"/>
+      <c r="D341" s="26"/>
+      <c r="E341" s="26"/>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A342" s="26"/>
+      <c r="B342" s="26"/>
+      <c r="C342" s="26"/>
+      <c r="D342" s="26"/>
+      <c r="E342" s="26"/>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A343" s="26"/>
+      <c r="B343" s="26"/>
+      <c r="C343" s="26"/>
+      <c r="D343" s="26"/>
+      <c r="E343" s="26"/>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A344" s="26"/>
+      <c r="B344" s="26"/>
+      <c r="C344" s="26"/>
+      <c r="D344" s="26"/>
+      <c r="E344" s="26"/>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A345" s="26"/>
+      <c r="B345" s="26"/>
+      <c r="C345" s="26"/>
+      <c r="D345" s="26"/>
+      <c r="E345" s="26"/>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A346" s="26"/>
+      <c r="B346" s="26"/>
+      <c r="C346" s="26"/>
+      <c r="D346" s="26"/>
+      <c r="E346" s="26"/>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A347" s="26"/>
+      <c r="B347" s="26"/>
+      <c r="C347" s="26"/>
+      <c r="D347" s="26"/>
+      <c r="E347" s="26"/>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A348" s="26"/>
+      <c r="B348" s="26"/>
+      <c r="C348" s="26"/>
+      <c r="D348" s="26"/>
+      <c r="E348" s="26"/>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A349" s="26"/>
+      <c r="B349" s="26"/>
+      <c r="C349" s="26"/>
+      <c r="D349" s="26"/>
+      <c r="E349" s="26"/>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A350" s="26"/>
+      <c r="B350" s="26"/>
+      <c r="C350" s="26"/>
+      <c r="D350" s="26"/>
+      <c r="E350" s="26"/>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A351" s="26"/>
+      <c r="B351" s="26"/>
+      <c r="C351" s="26"/>
+      <c r="D351" s="26"/>
+      <c r="E351" s="26"/>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A352" s="26"/>
+      <c r="B352" s="26"/>
+      <c r="C352" s="26"/>
+      <c r="D352" s="26"/>
+      <c r="E352" s="26"/>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A353" s="26"/>
+      <c r="B353" s="26"/>
+      <c r="C353" s="26"/>
+      <c r="D353" s="26"/>
+      <c r="E353" s="26"/>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A354" s="26"/>
+      <c r="B354" s="26"/>
+      <c r="C354" s="26"/>
+      <c r="D354" s="26"/>
+      <c r="E354" s="26"/>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A355" s="26"/>
+      <c r="B355" s="26"/>
+      <c r="C355" s="26"/>
+      <c r="D355" s="26"/>
+      <c r="E355" s="26"/>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A356" s="26"/>
+      <c r="B356" s="26"/>
+      <c r="C356" s="26"/>
+      <c r="D356" s="26"/>
+      <c r="E356" s="26"/>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A357" s="26"/>
+      <c r="B357" s="26"/>
+      <c r="C357" s="26"/>
+      <c r="D357" s="26"/>
+      <c r="E357" s="26"/>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A358" s="26"/>
+      <c r="B358" s="26"/>
+      <c r="C358" s="26"/>
+      <c r="D358" s="26"/>
+      <c r="E358" s="26"/>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A359" s="26"/>
+      <c r="B359" s="26"/>
+      <c r="C359" s="26"/>
+      <c r="D359" s="26"/>
+      <c r="E359" s="26"/>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A360" s="26"/>
+      <c r="B360" s="26"/>
+      <c r="C360" s="26"/>
+      <c r="D360" s="26"/>
+      <c r="E360" s="26"/>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A361" s="26"/>
+      <c r="B361" s="26"/>
+      <c r="C361" s="26"/>
+      <c r="D361" s="26"/>
+      <c r="E361" s="26"/>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A362" s="26"/>
+      <c r="B362" s="26"/>
+      <c r="C362" s="26"/>
+      <c r="D362" s="26"/>
+      <c r="E362" s="26"/>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A363" s="26"/>
+      <c r="B363" s="26"/>
+      <c r="C363" s="26"/>
+      <c r="D363" s="26"/>
+      <c r="E363" s="26"/>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A364" s="26"/>
+      <c r="B364" s="26"/>
+      <c r="C364" s="26"/>
+      <c r="D364" s="26"/>
+      <c r="E364" s="26"/>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A365" s="26"/>
+      <c r="B365" s="26"/>
+      <c r="C365" s="26"/>
+      <c r="D365" s="26"/>
+      <c r="E365" s="26"/>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A366" s="26"/>
+      <c r="B366" s="26"/>
+      <c r="C366" s="26"/>
+      <c r="D366" s="26"/>
+      <c r="E366" s="26"/>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A367" s="26"/>
+      <c r="B367" s="26"/>
+      <c r="C367" s="26"/>
+      <c r="D367" s="26"/>
+      <c r="E367" s="26"/>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A368" s="26"/>
+      <c r="B368" s="26"/>
+      <c r="C368" s="26"/>
+      <c r="D368" s="26"/>
+      <c r="E368" s="26"/>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A369" s="26"/>
+      <c r="B369" s="26"/>
+      <c r="C369" s="26"/>
+      <c r="D369" s="26"/>
+      <c r="E369" s="26"/>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A370" s="26"/>
+      <c r="B370" s="26"/>
+      <c r="C370" s="26"/>
+      <c r="D370" s="26"/>
+      <c r="E370" s="26"/>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A371" s="26"/>
+      <c r="B371" s="26"/>
+      <c r="C371" s="26"/>
+      <c r="D371" s="26"/>
+      <c r="E371" s="26"/>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A372" s="26"/>
+      <c r="B372" s="26"/>
+      <c r="C372" s="26"/>
+      <c r="D372" s="26"/>
+      <c r="E372" s="26"/>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A373" s="26"/>
+      <c r="B373" s="26"/>
+      <c r="C373" s="26"/>
+      <c r="D373" s="26"/>
+      <c r="E373" s="26"/>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A374" s="26"/>
+      <c r="B374" s="26"/>
+      <c r="C374" s="26"/>
+      <c r="D374" s="26"/>
+      <c r="E374" s="26"/>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A375" s="26"/>
+      <c r="B375" s="26"/>
+      <c r="C375" s="26"/>
+      <c r="D375" s="26"/>
+      <c r="E375" s="26"/>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A376" s="26"/>
+      <c r="B376" s="26"/>
+      <c r="C376" s="26"/>
+      <c r="D376" s="26"/>
+      <c r="E376" s="26"/>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A377" s="26"/>
+      <c r="B377" s="26"/>
+      <c r="C377" s="26"/>
+      <c r="D377" s="26"/>
+      <c r="E377" s="26"/>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A378" s="26"/>
+      <c r="B378" s="26"/>
+      <c r="C378" s="26"/>
+      <c r="D378" s="26"/>
+      <c r="E378" s="26"/>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A379" s="26"/>
+      <c r="B379" s="26"/>
+      <c r="C379" s="26"/>
+      <c r="D379" s="26"/>
+      <c r="E379" s="26"/>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A380" s="26"/>
+      <c r="B380" s="26"/>
+      <c r="C380" s="26"/>
+      <c r="D380" s="26"/>
+      <c r="E380" s="26"/>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A381" s="26"/>
+      <c r="B381" s="26"/>
+      <c r="C381" s="26"/>
+      <c r="D381" s="26"/>
+      <c r="E381" s="26"/>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A382" s="26"/>
+      <c r="B382" s="26"/>
+      <c r="C382" s="26"/>
+      <c r="D382" s="26"/>
+      <c r="E382" s="26"/>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A383" s="26"/>
+      <c r="B383" s="26"/>
+      <c r="C383" s="26"/>
+      <c r="D383" s="26"/>
+      <c r="E383" s="26"/>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A384" s="26"/>
+      <c r="B384" s="26"/>
+      <c r="C384" s="26"/>
+      <c r="D384" s="26"/>
+      <c r="E384" s="26"/>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A385" s="26"/>
+      <c r="B385" s="26"/>
+      <c r="C385" s="26"/>
+      <c r="D385" s="26"/>
+      <c r="E385" s="26"/>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A386" s="26"/>
+      <c r="B386" s="26"/>
+      <c r="C386" s="26"/>
+      <c r="D386" s="26"/>
+      <c r="E386" s="26"/>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A387" s="26"/>
+      <c r="B387" s="26"/>
+      <c r="C387" s="26"/>
+      <c r="D387" s="26"/>
+      <c r="E387" s="26"/>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A388" s="26"/>
+      <c r="B388" s="26"/>
+      <c r="C388" s="26"/>
+      <c r="D388" s="26"/>
+      <c r="E388" s="26"/>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A389" s="26"/>
+      <c r="B389" s="26"/>
+      <c r="C389" s="26"/>
+      <c r="D389" s="26"/>
+      <c r="E389" s="26"/>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A390" s="26"/>
+      <c r="B390" s="26"/>
+      <c r="C390" s="26"/>
+      <c r="D390" s="26"/>
+      <c r="E390" s="26"/>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A391" s="26"/>
+      <c r="B391" s="26"/>
+      <c r="C391" s="26"/>
+      <c r="D391" s="26"/>
+      <c r="E391" s="26"/>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A392" s="26"/>
+      <c r="B392" s="26"/>
+      <c r="C392" s="26"/>
+      <c r="D392" s="26"/>
+      <c r="E392" s="26"/>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A393" s="26"/>
+      <c r="B393" s="26"/>
+      <c r="C393" s="26"/>
+      <c r="D393" s="26"/>
+      <c r="E393" s="26"/>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A394" s="26"/>
+      <c r="B394" s="26"/>
+      <c r="C394" s="26"/>
+      <c r="D394" s="26"/>
+      <c r="E394" s="26"/>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A395" s="26"/>
+      <c r="B395" s="26"/>
+      <c r="C395" s="26"/>
+      <c r="D395" s="26"/>
+      <c r="E395" s="26"/>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A396" s="26"/>
+      <c r="B396" s="26"/>
+      <c r="C396" s="26"/>
+      <c r="D396" s="26"/>
+      <c r="E396" s="26"/>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A397" s="26"/>
+      <c r="B397" s="26"/>
+      <c r="C397" s="26"/>
+      <c r="D397" s="26"/>
+      <c r="E397" s="26"/>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A398" s="26"/>
+      <c r="B398" s="26"/>
+      <c r="C398" s="26"/>
+      <c r="D398" s="26"/>
+      <c r="E398" s="26"/>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A399" s="26"/>
+      <c r="B399" s="26"/>
+      <c r="C399" s="26"/>
+      <c r="D399" s="26"/>
+      <c r="E399" s="26"/>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A400" s="26"/>
+      <c r="B400" s="26"/>
+      <c r="C400" s="26"/>
+      <c r="D400" s="26"/>
+      <c r="E400" s="26"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2047,7 +4142,7 @@
   <dimension ref="A2:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2287,8 +4382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2609,8 +4704,8 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="str">
-        <f ca="1">CELL("address", Trading!A100)</f>
-        <v>[SpotTrading.xlsx]Trading!$A$100</v>
+        <f ca="1">CELL("address", Trading!A400)</f>
+        <v>[SpotTrading.xlsx]Trading!$A$400</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2629,8 +4724,8 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="str">
-        <f ca="1">CELL("address", Trading!B100)</f>
-        <v>[SpotTrading.xlsx]Trading!$B$100</v>
+        <f ca="1">CELL("address", Trading!B400)</f>
+        <v>[SpotTrading.xlsx]Trading!$B$400</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2649,8 +4744,8 @@
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="str">
-        <f ca="1">CELL("address", Trading!C100)</f>
-        <v>[SpotTrading.xlsx]Trading!$C$100</v>
+        <f ca="1">CELL("address", Trading!C400)</f>
+        <v>[SpotTrading.xlsx]Trading!$C$400</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2669,8 +4764,8 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="str">
-        <f ca="1">CELL("address", Trading!D100)</f>
-        <v>[SpotTrading.xlsx]Trading!$D$100</v>
+        <f ca="1">CELL("address", Trading!D400)</f>
+        <v>[SpotTrading.xlsx]Trading!$D$400</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2689,8 +4784,8 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="str">
-        <f ca="1">CELL("address", Trading!E100)</f>
-        <v>[SpotTrading.xlsx]Trading!$E$100</v>
+        <f ca="1">CELL("address", Trading!E400)</f>
+        <v>[SpotTrading.xlsx]Trading!$E$400</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completed the sample trading application
</commit_message>
<xml_diff>
--- a/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
+++ b/Examples/SpotTrading/SpotTrading/Views/SpotTrading.xlsx
@@ -209,7 +209,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00;0.00"/>
+    <numFmt numFmtId="166" formatCode="[Blue]#,##0.00;[Red]\-#,##0.00;0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -407,10 +407,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
@@ -695,16 +695,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>283853</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>107827</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>102878</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>88777</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -727,7 +727,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7820025" y="2686050"/>
+          <a:off x="9467850" y="0"/>
           <a:ext cx="3779528" cy="1984252"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1191,7 +1191,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="24">
-        <f>SUM(E10:E100)</f>
+        <f>SUM(E10:E400)</f>
         <v>0</v>
       </c>
       <c r="G8" s="12" t="s">

</xml_diff>